<commit_message>
fix: wrong merge conflict handling
</commit_message>
<xml_diff>
--- a/test/official_test_case_1.xlsx
+++ b/test/official_test_case_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/limnaroline/forecasting-project/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern\WEHI\prod\forecasting-with-workday-project\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3775693A-982B-2A40-887B-6D4537C2D51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBE241E-1D04-46EC-8E83-46641D33F279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1900" windowWidth="29600" windowHeight="15920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funding" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>Source ID</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>E010</t>
+  </si>
+  <si>
+    <t>sam</t>
   </si>
 </sst>
 </file>
@@ -545,13 +548,13 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -594,7 +597,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -614,7 +617,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -634,7 +637,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -654,7 +657,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -674,7 +677,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -694,7 +697,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -714,7 +717,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -734,7 +737,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -754,7 +757,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -774,7 +777,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -794,7 +797,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -814,7 +817,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -834,7 +837,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -854,7 +857,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -885,12 +888,12 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -913,13 +916,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
       </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
@@ -930,13 +936,16 @@
         <v>45703</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
       </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
       <c r="D3" t="s">
         <v>17</v>
       </c>
@@ -947,13 +956,16 @@
         <v>45726</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>52</v>
       </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
@@ -964,13 +976,16 @@
         <v>45736</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>53</v>
       </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
       <c r="D5" t="s">
         <v>14</v>
       </c>
@@ -981,13 +996,16 @@
         <v>45762</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
       </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
       <c r="D6" t="s">
         <v>17</v>
       </c>
@@ -998,13 +1016,16 @@
         <v>45797</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>55</v>
       </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
@@ -1015,13 +1036,16 @@
         <v>45818</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>56</v>
       </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
@@ -1032,13 +1056,16 @@
         <v>45853</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>57</v>
       </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
       <c r="D9" t="s">
         <v>17</v>
       </c>
@@ -1049,13 +1076,16 @@
         <v>45889</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>58</v>
       </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
       <c r="D10" t="s">
         <v>20</v>
       </c>
@@ -1066,12 +1096,15 @@
         <v>45940</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>

</xml_diff>